<commit_message>
v1.4.6 add learning data from 20201116 and add static blocked word in code zone
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/pinyin/20200525.xlsx
+++ b/ai/assets/textbook/pinyin/20200525.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\pinyin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C41221-3A12-4891-BB35-32F8B1B11B50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D350431A-32AC-4484-92DD-0BCA060DCC03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29415" yWindow="525" windowWidth="27390" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25950" yWindow="2445" windowWidth="18750" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
   <si>
     <t>发言内容</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>{viplv5}{dt0-10-5-17}盯死盯死</t>
-  </si>
-  <si>
-    <t>{viplv5}{dt1-0-6-29}Tony</t>
   </si>
   <si>
     <t>{viplv2}{dt1-2-5-23}不会讲广东话</t>
@@ -1062,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B365"/>
+  <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="A218" sqref="A218"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1415,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="1">
@@ -1426,7 +1423,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="1">
@@ -1434,7 +1431,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="1">
@@ -1450,7 +1447,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B48" s="1">
@@ -1466,7 +1463,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="1">
@@ -1474,7 +1471,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B51" s="1">
@@ -1506,7 +1503,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B55" s="1">
@@ -1514,7 +1511,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B56" s="1">
@@ -1570,7 +1567,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B63" s="1">
@@ -1650,7 +1647,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="1">
@@ -1658,7 +1655,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B74" s="1">
@@ -1666,7 +1663,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B75" s="1">
@@ -1690,7 +1687,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B78" s="1">
@@ -1698,7 +1695,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B79" s="1">
@@ -1730,7 +1727,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B83" s="1">
@@ -1746,7 +1743,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B85" s="1">
@@ -1754,7 +1751,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B86" s="1">
@@ -1762,7 +1759,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B87" s="1">
@@ -1778,7 +1775,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B89" s="1">
@@ -1818,7 +1815,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B94" s="1">
@@ -1826,7 +1823,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B95" s="1">
@@ -1850,7 +1847,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B98" s="1">
@@ -1858,7 +1855,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B99" s="1">
@@ -1866,7 +1863,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B100" s="1">
@@ -1898,7 +1895,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B104" s="1">
@@ -1906,7 +1903,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="A105" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B105" s="1">
@@ -1914,7 +1911,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B106" s="1">
@@ -1962,7 +1959,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B112" s="1">
@@ -1970,7 +1967,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B113" s="1">
@@ -1978,7 +1975,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B114" s="1">
@@ -1994,7 +1991,7 @@
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="A116" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B116" s="1">
@@ -2002,7 +1999,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B117" s="1">
@@ -2018,7 +2015,7 @@
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B119" s="1">
@@ -2034,7 +2031,7 @@
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="A121" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B121" s="1">
@@ -2106,7 +2103,7 @@
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B130" s="1">
@@ -2114,7 +2111,7 @@
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B131" s="1">
@@ -2162,7 +2159,7 @@
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B137" s="1">
@@ -2170,7 +2167,7 @@
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
+      <c r="A138" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B138" s="1">
@@ -2194,7 +2191,7 @@
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
+      <c r="A141" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B141" s="1">
@@ -2202,7 +2199,7 @@
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="3" t="s">
+      <c r="A142" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B142" s="1">
@@ -2218,7 +2215,7 @@
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B144" s="1">
@@ -2226,7 +2223,7 @@
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B145" s="1">
@@ -2234,7 +2231,7 @@
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
+      <c r="A146" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B146" s="1">
@@ -2242,7 +2239,7 @@
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
+      <c r="A147" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B147" s="1">
@@ -2362,7 +2359,7 @@
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
+      <c r="A162" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B162" s="1">
@@ -2370,7 +2367,7 @@
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
+      <c r="A163" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B163" s="1">
@@ -2466,11 +2463,11 @@
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
+      <c r="A175" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B175" s="1">
-        <v>0</v>
+      <c r="B175">
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,7 +2611,7 @@
         <v>193</v>
       </c>
       <c r="B193">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -2622,7 +2619,7 @@
         <v>194</v>
       </c>
       <c r="B194">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -2723,7 +2720,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -2731,7 +2728,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -2802,12 +2799,7 @@
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B217">
-        <v>1</v>
-      </c>
+      <c r="A217" s="5"/>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="5"/>
@@ -3121,11 +3113,11 @@
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="5"/>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="5"/>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="2"/>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="2"/>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="2"/>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="2"/>
@@ -3142,14 +3134,14 @@
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="2"/>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="2"/>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="2"/>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="2"/>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="2"/>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358" s="2"/>
+      <c r="A358" s="6"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="6"/>
@@ -3157,11 +3149,8 @@
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="6"/>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="6"/>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="2"/>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{9007686D-7565-4E50-BF8F-1EB4B9B99C50}"/>

</xml_diff>